<commit_message>
docs: rename 2013018_TestDesign -> 20130118_TestDesign
</commit_message>
<xml_diff>
--- a/20130118_TestPlan.xlsx
+++ b/20130118_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHI THANH\Desktop\TESTER\20130118_DoChiThanh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\END\Tester\tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9180FFF-F5B3-46D3-9D6E-4003B1E3F239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32A53A9-863D-4A91-B082-5323428B3CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -3766,53 +3766,8 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3825,6 +3780,27 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3853,14 +3829,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3922,91 +3922,19 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="126" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="13" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4045,6 +3973,105 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4072,47 +4099,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="112" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="112" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="112" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="112" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="112" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -4131,6 +4119,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="112" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="112" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="112" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5013,7 +5013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -5061,13 +5061,13 @@
     <row r="2" spans="1:26" ht="72" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="214" t="s">
+      <c r="C2" s="235" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="216"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="237"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -5090,12 +5090,12 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="217"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="219"/>
+      <c r="B3" s="238"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="239"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="240"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -5121,11 +5121,11 @@
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="220" t="s">
+      <c r="C4" s="241" t="s">
         <v>190</v>
       </c>
-      <c r="D4" s="221"/>
-      <c r="E4" s="222"/>
+      <c r="D4" s="220"/>
+      <c r="E4" s="221"/>
       <c r="F4" s="7" t="s">
         <v>2</v>
       </c>
@@ -5157,11 +5157,11 @@
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="223" t="s">
+      <c r="C5" s="242" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="224"/>
-      <c r="E5" s="225"/>
+      <c r="D5" s="223"/>
+      <c r="E5" s="224"/>
       <c r="F5" s="10" t="s">
         <v>4</v>
       </c>
@@ -5193,11 +5193,11 @@
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="226" t="s">
+      <c r="C6" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="D6" s="227"/>
-      <c r="E6" s="228"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="245"/>
       <c r="F6" s="10" t="s">
         <v>6</v>
       </c>
@@ -5229,11 +5229,11 @@
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="229" t="s">
+      <c r="C7" s="225" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="230"/>
-      <c r="E7" s="231"/>
+      <c r="D7" s="215"/>
+      <c r="E7" s="216"/>
       <c r="F7" s="13" t="s">
         <v>9</v>
       </c>
@@ -5290,10 +5290,10 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="232" t="s">
+      <c r="B9" s="217" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="233"/>
+      <c r="C9" s="218"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -5332,10 +5332,10 @@
       <c r="E10" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="235" t="s">
+      <c r="F10" s="227" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="236"/>
+      <c r="G10" s="228"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -5368,8 +5368,8 @@
         <v>15</v>
       </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="237"/>
-      <c r="G11" s="238"/>
+      <c r="F11" s="229"/>
+      <c r="G11" s="230"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
@@ -5396,8 +5396,8 @@
       <c r="C12" s="167"/>
       <c r="D12" s="168"/>
       <c r="E12" s="169"/>
-      <c r="F12" s="239"/>
-      <c r="G12" s="240"/>
+      <c r="F12" s="231"/>
+      <c r="G12" s="232"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
@@ -5448,10 +5448,10 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="232" t="s">
+      <c r="B14" s="217" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="233"/>
+      <c r="C14" s="218"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -5481,12 +5481,12 @@
       <c r="B15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="241" t="s">
+      <c r="C15" s="233" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="221"/>
-      <c r="E15" s="221"/>
-      <c r="F15" s="222"/>
+      <c r="D15" s="220"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="221"/>
       <c r="G15" s="20" t="s">
         <v>19</v>
       </c>
@@ -5515,12 +5515,12 @@
       <c r="B16" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="242" t="s">
+      <c r="C16" s="234" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="224"/>
-      <c r="E16" s="224"/>
-      <c r="F16" s="225"/>
+      <c r="D16" s="223"/>
+      <c r="E16" s="223"/>
+      <c r="F16" s="224"/>
       <c r="G16" s="22"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -5547,12 +5547,12 @@
       <c r="B17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="234" t="s">
+      <c r="C17" s="226" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="224"/>
-      <c r="E17" s="224"/>
-      <c r="F17" s="225"/>
+      <c r="D17" s="223"/>
+      <c r="E17" s="223"/>
+      <c r="F17" s="224"/>
       <c r="G17" s="22"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -5579,12 +5579,12 @@
       <c r="B18" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="234" t="s">
+      <c r="C18" s="226" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="224"/>
-      <c r="E18" s="224"/>
-      <c r="F18" s="225"/>
+      <c r="D18" s="223"/>
+      <c r="E18" s="223"/>
+      <c r="F18" s="224"/>
       <c r="G18" s="22"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -5611,12 +5611,12 @@
       <c r="B19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="234" t="s">
+      <c r="C19" s="226" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="224"/>
-      <c r="E19" s="224"/>
-      <c r="F19" s="225"/>
+      <c r="D19" s="223"/>
+      <c r="E19" s="223"/>
+      <c r="F19" s="224"/>
       <c r="G19" s="22"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -5643,12 +5643,12 @@
       <c r="B20" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="234" t="s">
+      <c r="C20" s="226" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="224"/>
-      <c r="E20" s="224"/>
-      <c r="F20" s="225"/>
+      <c r="D20" s="223"/>
+      <c r="E20" s="223"/>
+      <c r="F20" s="224"/>
       <c r="G20" s="22"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -5675,12 +5675,12 @@
       <c r="B21" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="243" t="s">
+      <c r="C21" s="214" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="230"/>
-      <c r="E21" s="230"/>
-      <c r="F21" s="231"/>
+      <c r="D21" s="215"/>
+      <c r="E21" s="215"/>
+      <c r="F21" s="216"/>
       <c r="G21" s="25" t="s">
         <v>32</v>
       </c>
@@ -5734,10 +5734,10 @@
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1">
       <c r="A23" s="26"/>
-      <c r="B23" s="232" t="s">
+      <c r="B23" s="217" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="233"/>
+      <c r="C23" s="218"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
@@ -5764,12 +5764,12 @@
     </row>
     <row r="24" spans="1:26" ht="18" customHeight="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="244" t="s">
+      <c r="B24" s="219" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="221"/>
-      <c r="D24" s="221"/>
-      <c r="E24" s="222"/>
+      <c r="C24" s="220"/>
+      <c r="D24" s="220"/>
+      <c r="E24" s="221"/>
       <c r="F24" s="14" t="s">
         <v>7</v>
       </c>
@@ -5798,12 +5798,12 @@
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1">
       <c r="A25" s="15"/>
-      <c r="B25" s="245" t="s">
+      <c r="B25" s="222" t="s">
         <v>191</v>
       </c>
-      <c r="C25" s="224"/>
-      <c r="D25" s="224"/>
-      <c r="E25" s="225"/>
+      <c r="C25" s="223"/>
+      <c r="D25" s="223"/>
+      <c r="E25" s="224"/>
       <c r="F25" s="30" t="s">
         <v>35</v>
       </c>
@@ -5830,10 +5830,10 @@
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1">
       <c r="A26" s="15"/>
-      <c r="B26" s="245"/>
-      <c r="C26" s="224"/>
-      <c r="D26" s="224"/>
-      <c r="E26" s="225"/>
+      <c r="B26" s="222"/>
+      <c r="C26" s="223"/>
+      <c r="D26" s="223"/>
+      <c r="E26" s="224"/>
       <c r="F26" s="31"/>
       <c r="G26" s="22"/>
       <c r="H26" s="15"/>
@@ -12205,11 +12205,11 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="C18:F18"/>
@@ -12222,11 +12222,11 @@
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -20041,21 +20041,21 @@
       <c r="A6" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="283" t="s">
+      <c r="B6" s="268" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="284"/>
-      <c r="D6" s="278" t="s">
+      <c r="C6" s="288"/>
+      <c r="D6" s="283" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="284"/>
+      <c r="E6" s="288"/>
       <c r="F6" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="278" t="s">
+      <c r="G6" s="283" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="279"/>
+      <c r="H6" s="270"/>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
@@ -20079,17 +20079,17 @@
       <c r="A7" s="64">
         <v>1</v>
       </c>
-      <c r="B7" s="280" t="s">
+      <c r="B7" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="268"/>
-      <c r="D7" s="280"/>
-      <c r="E7" s="268"/>
+      <c r="C7" s="285"/>
+      <c r="D7" s="291"/>
+      <c r="E7" s="285"/>
       <c r="F7" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="287"/>
-      <c r="H7" s="270"/>
+      <c r="G7" s="295"/>
+      <c r="H7" s="296"/>
       <c r="I7" s="32"/>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
@@ -20113,17 +20113,17 @@
       <c r="A8" s="64">
         <v>2</v>
       </c>
-      <c r="B8" s="280" t="s">
+      <c r="B8" s="291" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="268"/>
-      <c r="D8" s="281"/>
-      <c r="E8" s="268"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="292"/>
+      <c r="E8" s="285"/>
       <c r="F8" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="281"/>
-      <c r="H8" s="270"/>
+      <c r="G8" s="292"/>
+      <c r="H8" s="296"/>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
@@ -20147,17 +20147,17 @@
       <c r="A9" s="64">
         <v>3</v>
       </c>
-      <c r="B9" s="282" t="s">
+      <c r="B9" s="289" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="268"/>
-      <c r="D9" s="281"/>
-      <c r="E9" s="268"/>
+      <c r="C9" s="285"/>
+      <c r="D9" s="292"/>
+      <c r="E9" s="285"/>
       <c r="F9" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="281"/>
-      <c r="H9" s="270"/>
+      <c r="G9" s="292"/>
+      <c r="H9" s="296"/>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
@@ -20181,17 +20181,17 @@
       <c r="A10" s="64">
         <v>4</v>
       </c>
-      <c r="B10" s="282" t="s">
+      <c r="B10" s="289" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="268"/>
-      <c r="D10" s="281"/>
-      <c r="E10" s="268"/>
+      <c r="C10" s="285"/>
+      <c r="D10" s="292"/>
+      <c r="E10" s="285"/>
       <c r="F10" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="281"/>
-      <c r="H10" s="270"/>
+      <c r="G10" s="292"/>
+      <c r="H10" s="296"/>
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
@@ -20215,17 +20215,17 @@
       <c r="A11" s="64">
         <v>5</v>
       </c>
-      <c r="B11" s="280" t="s">
+      <c r="B11" s="291" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="268"/>
-      <c r="D11" s="281"/>
-      <c r="E11" s="268"/>
+      <c r="C11" s="285"/>
+      <c r="D11" s="292"/>
+      <c r="E11" s="285"/>
       <c r="F11" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="281"/>
-      <c r="H11" s="270"/>
+      <c r="G11" s="292"/>
+      <c r="H11" s="296"/>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
@@ -20249,17 +20249,17 @@
       <c r="A12" s="64">
         <v>6</v>
       </c>
-      <c r="B12" s="280" t="s">
+      <c r="B12" s="291" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="268"/>
-      <c r="D12" s="281"/>
-      <c r="E12" s="268"/>
+      <c r="C12" s="285"/>
+      <c r="D12" s="292"/>
+      <c r="E12" s="285"/>
       <c r="F12" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="281"/>
-      <c r="H12" s="270"/>
+      <c r="G12" s="292"/>
+      <c r="H12" s="296"/>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
@@ -20283,17 +20283,17 @@
       <c r="A13" s="64">
         <v>7</v>
       </c>
-      <c r="B13" s="288" t="s">
+      <c r="B13" s="298" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="286"/>
-      <c r="D13" s="285"/>
-      <c r="E13" s="286"/>
+      <c r="C13" s="294"/>
+      <c r="D13" s="293"/>
+      <c r="E13" s="294"/>
       <c r="F13" s="202" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="285"/>
-      <c r="H13" s="274"/>
+      <c r="G13" s="293"/>
+      <c r="H13" s="297"/>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
@@ -20405,10 +20405,10 @@
       <c r="A17" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="283" t="s">
+      <c r="B17" s="268" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="284"/>
+      <c r="C17" s="288"/>
       <c r="D17" s="63" t="s">
         <v>77</v>
       </c>
@@ -20418,10 +20418,10 @@
       <c r="F17" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="278" t="s">
+      <c r="G17" s="283" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="279"/>
+      <c r="H17" s="270"/>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
@@ -20445,10 +20445,10 @@
       <c r="A18" s="65">
         <v>1</v>
       </c>
-      <c r="B18" s="282" t="s">
+      <c r="B18" s="289" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="268"/>
+      <c r="C18" s="285"/>
       <c r="D18" s="67">
         <v>45594</v>
       </c>
@@ -20458,10 +20458,10 @@
       <c r="F18" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="266" t="s">
+      <c r="G18" s="284" t="s">
         <v>83</v>
       </c>
-      <c r="H18" s="268"/>
+      <c r="H18" s="285"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
@@ -20485,10 +20485,10 @@
       <c r="A19" s="68">
         <v>2</v>
       </c>
-      <c r="B19" s="289" t="s">
+      <c r="B19" s="290" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="290"/>
+      <c r="C19" s="287"/>
       <c r="D19" s="67">
         <v>45594</v>
       </c>
@@ -20498,8 +20498,8 @@
       <c r="F19" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="291"/>
-      <c r="H19" s="290"/>
+      <c r="G19" s="286"/>
+      <c r="H19" s="287"/>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
@@ -20523,10 +20523,10 @@
       <c r="A20" s="65">
         <v>3</v>
       </c>
-      <c r="B20" s="282" t="s">
+      <c r="B20" s="289" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="268"/>
+      <c r="C20" s="285"/>
       <c r="D20" s="67">
         <v>45594</v>
       </c>
@@ -20536,8 +20536,8 @@
       <c r="F20" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="G20" s="266"/>
-      <c r="H20" s="268"/>
+      <c r="G20" s="284"/>
+      <c r="H20" s="285"/>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
@@ -20561,10 +20561,10 @@
       <c r="A21" s="65">
         <v>4</v>
       </c>
-      <c r="B21" s="282" t="s">
+      <c r="B21" s="289" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="268"/>
+      <c r="C21" s="285"/>
       <c r="D21" s="67">
         <v>45594</v>
       </c>
@@ -20574,8 +20574,8 @@
       <c r="F21" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="266"/>
-      <c r="H21" s="268"/>
+      <c r="G21" s="284"/>
+      <c r="H21" s="285"/>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
@@ -20687,19 +20687,19 @@
       <c r="A25" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="295" t="s">
+      <c r="B25" s="271" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="225"/>
+      <c r="C25" s="224"/>
       <c r="D25" s="250" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="224"/>
-      <c r="F25" s="225"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="224"/>
       <c r="G25" s="250" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="225"/>
+      <c r="H25" s="224"/>
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
@@ -20723,13 +20723,13 @@
       <c r="A26" s="70">
         <v>1</v>
       </c>
-      <c r="B26" s="296"/>
-      <c r="C26" s="297"/>
-      <c r="D26" s="300"/>
-      <c r="E26" s="301"/>
-      <c r="F26" s="297"/>
-      <c r="G26" s="300"/>
-      <c r="H26" s="297"/>
+      <c r="B26" s="272"/>
+      <c r="C26" s="273"/>
+      <c r="D26" s="276"/>
+      <c r="E26" s="277"/>
+      <c r="F26" s="273"/>
+      <c r="G26" s="276"/>
+      <c r="H26" s="273"/>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
@@ -20753,13 +20753,13 @@
       <c r="A27" s="71">
         <v>2</v>
       </c>
-      <c r="B27" s="298"/>
-      <c r="C27" s="299"/>
-      <c r="D27" s="302"/>
-      <c r="E27" s="303"/>
-      <c r="F27" s="299"/>
-      <c r="G27" s="304"/>
-      <c r="H27" s="299"/>
+      <c r="B27" s="274"/>
+      <c r="C27" s="275"/>
+      <c r="D27" s="278"/>
+      <c r="E27" s="279"/>
+      <c r="F27" s="275"/>
+      <c r="G27" s="280"/>
+      <c r="H27" s="275"/>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
@@ -20783,13 +20783,13 @@
       <c r="A28" s="72">
         <v>3</v>
       </c>
-      <c r="B28" s="292"/>
-      <c r="C28" s="293"/>
-      <c r="D28" s="305"/>
-      <c r="E28" s="306"/>
-      <c r="F28" s="293"/>
-      <c r="G28" s="305"/>
-      <c r="H28" s="293"/>
+      <c r="B28" s="266"/>
+      <c r="C28" s="267"/>
+      <c r="D28" s="281"/>
+      <c r="E28" s="282"/>
+      <c r="F28" s="267"/>
+      <c r="G28" s="281"/>
+      <c r="H28" s="267"/>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
@@ -20901,19 +20901,19 @@
       <c r="A32" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="283" t="s">
+      <c r="B32" s="268" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="294"/>
-      <c r="D32" s="279"/>
-      <c r="E32" s="283" t="s">
+      <c r="C32" s="269"/>
+      <c r="D32" s="270"/>
+      <c r="E32" s="268" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="279"/>
-      <c r="G32" s="283" t="s">
+      <c r="F32" s="270"/>
+      <c r="G32" s="268" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="279"/>
+      <c r="H32" s="270"/>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
       <c r="K32" s="32"/>
@@ -20937,19 +20937,19 @@
       <c r="A33" s="77">
         <v>1</v>
       </c>
-      <c r="B33" s="266" t="s">
+      <c r="B33" s="284" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="267"/>
-      <c r="D33" s="268"/>
-      <c r="E33" s="266" t="s">
+      <c r="C33" s="300"/>
+      <c r="D33" s="285"/>
+      <c r="E33" s="284" t="s">
         <v>97</v>
       </c>
-      <c r="F33" s="268"/>
-      <c r="G33" s="266" t="s">
+      <c r="F33" s="285"/>
+      <c r="G33" s="284" t="s">
         <v>98</v>
       </c>
-      <c r="H33" s="268"/>
+      <c r="H33" s="285"/>
       <c r="I33" s="33"/>
       <c r="J33" s="33"/>
       <c r="K33" s="33"/>
@@ -20973,19 +20973,19 @@
       <c r="A34" s="77">
         <v>2</v>
       </c>
-      <c r="B34" s="266" t="s">
+      <c r="B34" s="284" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="267"/>
-      <c r="D34" s="268"/>
-      <c r="E34" s="266" t="s">
+      <c r="C34" s="300"/>
+      <c r="D34" s="285"/>
+      <c r="E34" s="284" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="268"/>
-      <c r="G34" s="266" t="s">
+      <c r="F34" s="285"/>
+      <c r="G34" s="284" t="s">
         <v>101</v>
       </c>
-      <c r="H34" s="268"/>
+      <c r="H34" s="285"/>
       <c r="I34" s="33"/>
       <c r="J34" s="33"/>
       <c r="K34" s="33"/>
@@ -21009,19 +21009,19 @@
       <c r="A35" s="77">
         <v>3</v>
       </c>
-      <c r="B35" s="266" t="s">
+      <c r="B35" s="284" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="267"/>
-      <c r="D35" s="268"/>
-      <c r="E35" s="266" t="s">
+      <c r="C35" s="300"/>
+      <c r="D35" s="285"/>
+      <c r="E35" s="284" t="s">
         <v>103</v>
       </c>
-      <c r="F35" s="268"/>
-      <c r="G35" s="266" t="s">
+      <c r="F35" s="285"/>
+      <c r="G35" s="284" t="s">
         <v>104</v>
       </c>
-      <c r="H35" s="268"/>
+      <c r="H35" s="285"/>
       <c r="I35" s="33"/>
       <c r="J35" s="33"/>
       <c r="K35" s="33"/>
@@ -21045,19 +21045,19 @@
       <c r="A36" s="77">
         <v>4</v>
       </c>
-      <c r="B36" s="266" t="s">
+      <c r="B36" s="284" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="267"/>
-      <c r="D36" s="268"/>
-      <c r="E36" s="266" t="s">
+      <c r="C36" s="300"/>
+      <c r="D36" s="285"/>
+      <c r="E36" s="284" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="268"/>
-      <c r="G36" s="266" t="s">
+      <c r="F36" s="285"/>
+      <c r="G36" s="284" t="s">
         <v>107</v>
       </c>
-      <c r="H36" s="268"/>
+      <c r="H36" s="285"/>
       <c r="I36" s="33"/>
       <c r="J36" s="33"/>
       <c r="K36" s="33"/>
@@ -21081,19 +21081,19 @@
       <c r="A37" s="77">
         <v>5</v>
       </c>
-      <c r="B37" s="266" t="s">
+      <c r="B37" s="284" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="267"/>
-      <c r="D37" s="268"/>
-      <c r="E37" s="266" t="s">
+      <c r="C37" s="300"/>
+      <c r="D37" s="285"/>
+      <c r="E37" s="284" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="268"/>
-      <c r="G37" s="266" t="s">
+      <c r="F37" s="285"/>
+      <c r="G37" s="284" t="s">
         <v>109</v>
       </c>
-      <c r="H37" s="268"/>
+      <c r="H37" s="285"/>
       <c r="I37" s="33"/>
       <c r="J37" s="33"/>
       <c r="K37" s="33"/>
@@ -21205,17 +21205,17 @@
       <c r="A41" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="271" t="s">
+      <c r="B41" s="301" t="s">
         <v>112</v>
       </c>
-      <c r="C41" s="225"/>
+      <c r="C41" s="224"/>
       <c r="D41" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="224"/>
-      <c r="F41" s="224"/>
-      <c r="G41" s="224"/>
-      <c r="H41" s="225"/>
+      <c r="E41" s="223"/>
+      <c r="F41" s="223"/>
+      <c r="G41" s="223"/>
+      <c r="H41" s="224"/>
       <c r="I41" s="32"/>
       <c r="J41" s="32"/>
       <c r="K41" s="32"/>
@@ -21239,13 +21239,13 @@
       <c r="A42" s="79">
         <v>1</v>
       </c>
-      <c r="B42" s="272"/>
-      <c r="C42" s="270"/>
-      <c r="D42" s="272"/>
-      <c r="E42" s="267"/>
-      <c r="F42" s="267"/>
-      <c r="G42" s="267"/>
-      <c r="H42" s="270"/>
+      <c r="B42" s="302"/>
+      <c r="C42" s="296"/>
+      <c r="D42" s="302"/>
+      <c r="E42" s="300"/>
+      <c r="F42" s="300"/>
+      <c r="G42" s="300"/>
+      <c r="H42" s="296"/>
       <c r="I42" s="32"/>
       <c r="J42" s="32"/>
       <c r="K42" s="32"/>
@@ -21269,13 +21269,13 @@
       <c r="A43" s="80">
         <v>2</v>
       </c>
-      <c r="B43" s="273"/>
-      <c r="C43" s="274"/>
-      <c r="D43" s="273"/>
-      <c r="E43" s="277"/>
-      <c r="F43" s="277"/>
-      <c r="G43" s="277"/>
-      <c r="H43" s="274"/>
+      <c r="B43" s="303"/>
+      <c r="C43" s="297"/>
+      <c r="D43" s="303"/>
+      <c r="E43" s="306"/>
+      <c r="F43" s="306"/>
+      <c r="G43" s="306"/>
+      <c r="H43" s="297"/>
       <c r="I43" s="32"/>
       <c r="J43" s="32"/>
       <c r="K43" s="32"/>
@@ -21390,11 +21390,11 @@
       <c r="B47" s="250" t="s">
         <v>115</v>
       </c>
-      <c r="C47" s="225"/>
+      <c r="C47" s="224"/>
       <c r="D47" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="225"/>
+      <c r="E47" s="224"/>
       <c r="F47" s="81" t="s">
         <v>39</v>
       </c>
@@ -21427,10 +21427,10 @@
       <c r="A48" s="82">
         <v>1</v>
       </c>
-      <c r="B48" s="275"/>
-      <c r="C48" s="276"/>
-      <c r="D48" s="275"/>
-      <c r="E48" s="276"/>
+      <c r="B48" s="304"/>
+      <c r="C48" s="305"/>
+      <c r="D48" s="304"/>
+      <c r="E48" s="305"/>
       <c r="F48" s="83"/>
       <c r="G48" s="84"/>
       <c r="H48" s="84"/>
@@ -21457,10 +21457,10 @@
       <c r="A49" s="85">
         <v>2</v>
       </c>
-      <c r="B49" s="269"/>
-      <c r="C49" s="270"/>
-      <c r="D49" s="269"/>
-      <c r="E49" s="270"/>
+      <c r="B49" s="299"/>
+      <c r="C49" s="296"/>
+      <c r="D49" s="299"/>
+      <c r="E49" s="296"/>
       <c r="F49" s="86"/>
       <c r="G49" s="84"/>
       <c r="H49" s="84"/>
@@ -21487,10 +21487,10 @@
       <c r="A50" s="82">
         <v>3</v>
       </c>
-      <c r="B50" s="269"/>
-      <c r="C50" s="270"/>
-      <c r="D50" s="269"/>
-      <c r="E50" s="270"/>
+      <c r="B50" s="299"/>
+      <c r="C50" s="296"/>
+      <c r="D50" s="299"/>
+      <c r="E50" s="296"/>
       <c r="F50" s="86"/>
       <c r="G50" s="84"/>
       <c r="H50" s="84"/>
@@ -27865,31 +27865,43 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
@@ -27906,43 +27918,31 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -28240,20 +28240,20 @@
       <c r="B10" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="308" t="s">
+      <c r="C10" s="317" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="310" t="s">
+      <c r="D10" s="319" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="310" t="s">
+      <c r="E10" s="319" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="311" t="s">
+      <c r="F10" s="320" t="s">
         <v>126</v>
       </c>
-      <c r="G10" s="312"/>
-      <c r="H10" s="314"/>
+      <c r="G10" s="321"/>
+      <c r="H10" s="323"/>
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
@@ -28278,12 +28278,12 @@
       <c r="B11" s="89" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="309"/>
-      <c r="D11" s="309"/>
-      <c r="E11" s="309"/>
-      <c r="F11" s="309"/>
-      <c r="G11" s="313"/>
-      <c r="H11" s="315"/>
+      <c r="C11" s="318"/>
+      <c r="D11" s="318"/>
+      <c r="E11" s="318"/>
+      <c r="F11" s="318"/>
+      <c r="G11" s="322"/>
+      <c r="H11" s="324"/>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
@@ -28532,16 +28532,16 @@
       <c r="B19" s="250" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="225"/>
+      <c r="C19" s="224"/>
       <c r="D19" s="250" t="s">
         <v>135</v>
       </c>
-      <c r="E19" s="224"/>
-      <c r="F19" s="307"/>
+      <c r="E19" s="223"/>
+      <c r="F19" s="316"/>
       <c r="G19" s="250" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="225"/>
+      <c r="H19" s="224"/>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
@@ -28563,17 +28563,17 @@
     </row>
     <row r="20" spans="1:26" ht="51" customHeight="1">
       <c r="A20" s="33"/>
-      <c r="B20" s="316" t="s">
+      <c r="B20" s="311" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="225"/>
-      <c r="D20" s="317" t="s">
+      <c r="C20" s="224"/>
+      <c r="D20" s="313" t="s">
         <v>208</v>
       </c>
-      <c r="E20" s="224"/>
-      <c r="F20" s="224"/>
-      <c r="G20" s="318"/>
-      <c r="H20" s="225"/>
+      <c r="E20" s="223"/>
+      <c r="F20" s="223"/>
+      <c r="G20" s="315"/>
+      <c r="H20" s="224"/>
       <c r="I20" s="33"/>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
@@ -28717,13 +28717,13 @@
       <c r="C25" s="250" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="224"/>
-      <c r="E25" s="224"/>
-      <c r="F25" s="225"/>
-      <c r="G25" s="271" t="s">
+      <c r="D25" s="223"/>
+      <c r="E25" s="223"/>
+      <c r="F25" s="224"/>
+      <c r="G25" s="301" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="225"/>
+      <c r="H25" s="224"/>
       <c r="I25" s="33"/>
       <c r="J25" s="33"/>
       <c r="K25" s="33"/>
@@ -28748,16 +28748,16 @@
       <c r="B26" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="319" t="s">
+      <c r="C26" s="307" t="s">
         <v>141</v>
       </c>
-      <c r="D26" s="224"/>
-      <c r="E26" s="224"/>
-      <c r="F26" s="225"/>
-      <c r="G26" s="320" t="s">
+      <c r="D26" s="223"/>
+      <c r="E26" s="223"/>
+      <c r="F26" s="224"/>
+      <c r="G26" s="308" t="s">
         <v>142</v>
       </c>
-      <c r="H26" s="225"/>
+      <c r="H26" s="224"/>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
@@ -28782,14 +28782,14 @@
       <c r="B27" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="316" t="s">
+      <c r="C27" s="311" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="224"/>
-      <c r="E27" s="224"/>
-      <c r="F27" s="225"/>
-      <c r="G27" s="323"/>
-      <c r="H27" s="225"/>
+      <c r="D27" s="223"/>
+      <c r="E27" s="223"/>
+      <c r="F27" s="224"/>
+      <c r="G27" s="312"/>
+      <c r="H27" s="224"/>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
@@ -28814,14 +28814,14 @@
       <c r="B28" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="317" t="s">
+      <c r="C28" s="313" t="s">
         <v>207</v>
       </c>
-      <c r="D28" s="224"/>
-      <c r="E28" s="224"/>
-      <c r="F28" s="225"/>
-      <c r="G28" s="320"/>
-      <c r="H28" s="225"/>
+      <c r="D28" s="223"/>
+      <c r="E28" s="223"/>
+      <c r="F28" s="224"/>
+      <c r="G28" s="308"/>
+      <c r="H28" s="224"/>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
@@ -28846,14 +28846,14 @@
       <c r="B29" s="97" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="324" t="s">
+      <c r="C29" s="314" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="224"/>
-      <c r="E29" s="224"/>
-      <c r="F29" s="225"/>
-      <c r="G29" s="322"/>
-      <c r="H29" s="225"/>
+      <c r="D29" s="223"/>
+      <c r="E29" s="223"/>
+      <c r="F29" s="224"/>
+      <c r="G29" s="310"/>
+      <c r="H29" s="224"/>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
       <c r="K29" s="32"/>
@@ -28878,14 +28878,14 @@
       <c r="B30" s="98" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="321" t="s">
+      <c r="C30" s="309" t="s">
         <v>149</v>
       </c>
-      <c r="D30" s="224"/>
-      <c r="E30" s="224"/>
-      <c r="F30" s="225"/>
-      <c r="G30" s="322"/>
-      <c r="H30" s="225"/>
+      <c r="D30" s="223"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="224"/>
+      <c r="G30" s="310"/>
+      <c r="H30" s="224"/>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
       <c r="K30" s="32"/>
@@ -28910,14 +28910,14 @@
       <c r="B31" s="97" t="s">
         <v>150</v>
       </c>
-      <c r="C31" s="320" t="s">
+      <c r="C31" s="308" t="s">
         <v>151</v>
       </c>
-      <c r="D31" s="224"/>
-      <c r="E31" s="224"/>
-      <c r="F31" s="225"/>
-      <c r="G31" s="322"/>
-      <c r="H31" s="225"/>
+      <c r="D31" s="223"/>
+      <c r="E31" s="223"/>
+      <c r="F31" s="224"/>
+      <c r="G31" s="310"/>
+      <c r="H31" s="224"/>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
       <c r="K31" s="32"/>
@@ -35308,6 +35308,20 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="C30:F30"/>
@@ -35320,20 +35334,6 @@
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -35514,15 +35514,15 @@
       <c r="C6" s="195" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="325" t="s">
+      <c r="D6" s="332" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="326"/>
-      <c r="F6" s="326"/>
-      <c r="G6" s="326"/>
-      <c r="H6" s="326"/>
-      <c r="I6" s="326"/>
-      <c r="J6" s="326"/>
+      <c r="E6" s="333"/>
+      <c r="F6" s="333"/>
+      <c r="G6" s="333"/>
+      <c r="H6" s="333"/>
+      <c r="I6" s="333"/>
+      <c r="J6" s="333"/>
       <c r="K6" s="32"/>
       <c r="L6" s="32"/>
       <c r="M6" s="32"/>
@@ -35550,15 +35550,15 @@
       <c r="C7" s="196" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="327" t="s">
+      <c r="D7" s="325" t="s">
         <v>226</v>
       </c>
-      <c r="E7" s="328"/>
-      <c r="F7" s="328"/>
-      <c r="G7" s="328"/>
-      <c r="H7" s="328"/>
-      <c r="I7" s="328"/>
-      <c r="J7" s="329"/>
+      <c r="E7" s="334"/>
+      <c r="F7" s="334"/>
+      <c r="G7" s="334"/>
+      <c r="H7" s="334"/>
+      <c r="I7" s="334"/>
+      <c r="J7" s="335"/>
       <c r="K7" s="32"/>
       <c r="L7" s="32"/>
       <c r="M7" s="32"/>
@@ -35586,15 +35586,15 @@
       <c r="C8" s="196" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="327" t="s">
+      <c r="D8" s="325" t="s">
         <v>227</v>
       </c>
-      <c r="E8" s="330"/>
-      <c r="F8" s="330"/>
-      <c r="G8" s="330"/>
-      <c r="H8" s="330"/>
-      <c r="I8" s="330"/>
-      <c r="J8" s="331"/>
+      <c r="E8" s="326"/>
+      <c r="F8" s="326"/>
+      <c r="G8" s="326"/>
+      <c r="H8" s="326"/>
+      <c r="I8" s="326"/>
+      <c r="J8" s="327"/>
       <c r="K8" s="32"/>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
@@ -35622,15 +35622,15 @@
       <c r="C9" s="196" t="s">
         <v>158</v>
       </c>
-      <c r="D9" s="327" t="s">
+      <c r="D9" s="325" t="s">
         <v>228</v>
       </c>
-      <c r="E9" s="330"/>
-      <c r="F9" s="330"/>
-      <c r="G9" s="330"/>
-      <c r="H9" s="330"/>
-      <c r="I9" s="330"/>
-      <c r="J9" s="331"/>
+      <c r="E9" s="326"/>
+      <c r="F9" s="326"/>
+      <c r="G9" s="326"/>
+      <c r="H9" s="326"/>
+      <c r="I9" s="326"/>
+      <c r="J9" s="327"/>
       <c r="K9" s="32"/>
       <c r="L9" s="32"/>
       <c r="M9" s="32"/>
@@ -35658,15 +35658,15 @@
       <c r="C10" s="196" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="327" t="s">
+      <c r="D10" s="325" t="s">
         <v>229</v>
       </c>
-      <c r="E10" s="330"/>
-      <c r="F10" s="330"/>
-      <c r="G10" s="330"/>
-      <c r="H10" s="330"/>
-      <c r="I10" s="330"/>
-      <c r="J10" s="331"/>
+      <c r="E10" s="326"/>
+      <c r="F10" s="326"/>
+      <c r="G10" s="326"/>
+      <c r="H10" s="326"/>
+      <c r="I10" s="326"/>
+      <c r="J10" s="327"/>
       <c r="K10" s="32"/>
       <c r="L10" s="32"/>
       <c r="M10" s="32"/>
@@ -35694,15 +35694,15 @@
       <c r="C11" s="196" t="s">
         <v>158</v>
       </c>
-      <c r="D11" s="327" t="s">
+      <c r="D11" s="325" t="s">
         <v>230</v>
       </c>
-      <c r="E11" s="330"/>
-      <c r="F11" s="330"/>
-      <c r="G11" s="330"/>
-      <c r="H11" s="330"/>
-      <c r="I11" s="330"/>
-      <c r="J11" s="331"/>
+      <c r="E11" s="326"/>
+      <c r="F11" s="326"/>
+      <c r="G11" s="326"/>
+      <c r="H11" s="326"/>
+      <c r="I11" s="326"/>
+      <c r="J11" s="327"/>
       <c r="K11" s="32"/>
       <c r="L11" s="32"/>
       <c r="M11" s="32"/>
@@ -35811,7 +35811,7 @@
       <c r="D15" s="250" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="225"/>
+      <c r="E15" s="224"/>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
@@ -35842,10 +35842,10 @@
       <c r="C16" s="105">
         <v>45591</v>
       </c>
-      <c r="D16" s="334">
+      <c r="D16" s="330">
         <v>45597</v>
       </c>
-      <c r="E16" s="335"/>
+      <c r="E16" s="331"/>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
@@ -35876,10 +35876,10 @@
       <c r="C17" s="108">
         <v>45591</v>
       </c>
-      <c r="D17" s="332">
+      <c r="D17" s="328">
         <v>45597</v>
       </c>
-      <c r="E17" s="270"/>
+      <c r="E17" s="296"/>
       <c r="F17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="32"/>
@@ -35908,8 +35908,8 @@
         <v>160</v>
       </c>
       <c r="C18" s="108"/>
-      <c r="D18" s="332"/>
-      <c r="E18" s="270"/>
+      <c r="D18" s="328"/>
+      <c r="E18" s="296"/>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
@@ -35938,8 +35938,8 @@
         <v>161</v>
       </c>
       <c r="C19" s="111"/>
-      <c r="D19" s="332"/>
-      <c r="E19" s="270"/>
+      <c r="D19" s="328"/>
+      <c r="E19" s="296"/>
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
@@ -35968,8 +35968,8 @@
         <v>162</v>
       </c>
       <c r="C20" s="108"/>
-      <c r="D20" s="332"/>
-      <c r="E20" s="270"/>
+      <c r="D20" s="328"/>
+      <c r="E20" s="296"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
@@ -35998,8 +35998,8 @@
         <v>163</v>
       </c>
       <c r="C21" s="116"/>
-      <c r="D21" s="333"/>
-      <c r="E21" s="274"/>
+      <c r="D21" s="329"/>
+      <c r="E21" s="297"/>
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
@@ -42328,6 +42328,11 @@
     <row r="995" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D10:J10"/>
     <mergeCell ref="D11:J11"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -42336,11 +42341,6 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D10:J10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B32" location="Detail Schedule!A1" display="Liên kết" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -42361,7 +42361,7 @@
   </sheetPr>
   <dimension ref="A1:AG985"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -42818,9 +42818,9 @@
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
       <c r="K11" s="336"/>
-      <c r="L11" s="218"/>
-      <c r="M11" s="218"/>
-      <c r="N11" s="233"/>
+      <c r="L11" s="239"/>
+      <c r="M11" s="239"/>
+      <c r="N11" s="218"/>
       <c r="O11" s="32"/>
       <c r="P11" s="32"/>
       <c r="Q11" s="32"/>

</xml_diff>